<commit_message>
al parecer funciona lo de revision de escaleras, pero esta re feo xd
</commit_message>
<xml_diff>
--- a/app/templates/template_rules_ladder.xlsx
+++ b/app/templates/template_rules_ladder.xlsx
@@ -94,7 +94,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">5.1</t>
+    <t xml:space="preserve">5.1.1</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -8759,7 +8759,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">4</t>
+      <t xml:space="preserve">4.1</t>
     </r>
   </si>
   <si>
@@ -9532,6 +9532,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -9822,7 +9823,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="87">
+  <borders count="85">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -9858,7 +9859,7 @@
       <right style="medium"/>
       <top style="medium"/>
       <bottom style="medium">
-        <color rgb="FF355163"/>
+        <color rgb="FF345260"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9880,7 +9881,7 @@
       </right>
       <top style="medium"/>
       <bottom style="medium">
-        <color rgb="FF3D5C6D"/>
+        <color rgb="FF3D5D6E"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9892,7 +9893,7 @@
         <color rgb="FF2B4F5F"/>
       </right>
       <top style="medium">
-        <color rgb="FF355163"/>
+        <color rgb="FF345260"/>
       </top>
       <bottom style="medium"/>
       <diagonal/>
@@ -9914,7 +9915,7 @@
       </left>
       <right/>
       <top style="medium">
-        <color rgb="FF3D5C6D"/>
+        <color rgb="FF3D5D6E"/>
       </top>
       <bottom style="medium">
         <color rgb="FF22495F"/>
@@ -10047,7 +10048,7 @@
         <color rgb="FF446578"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF223F4D"/>
+        <color rgb="FF233F4D"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10058,7 +10059,7 @@
         <color rgb="FF1D4457"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF355666"/>
+        <color rgb="FF365666"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10083,7 +10084,7 @@
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="medium">
-        <color rgb="FF34586A"/>
+        <color rgb="FF345967"/>
       </right>
       <top style="medium">
         <color rgb="FF2B4F64"/>
@@ -10093,10 +10094,10 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="medium">
-        <color rgb="FF34586A"/>
+        <color rgb="FF345967"/>
       </left>
       <right style="medium">
-        <color rgb="FF355666"/>
+        <color rgb="FF365666"/>
       </right>
       <top style="medium">
         <color rgb="FF2B4F64"/>
@@ -10152,7 +10153,7 @@
         <color rgb="FF284457"/>
       </left>
       <right style="medium">
-        <color rgb="FF23444F"/>
+        <color rgb="FF274452"/>
       </right>
       <top style="medium"/>
       <bottom style="medium">
@@ -10206,7 +10207,7 @@
         <color rgb="FF284457"/>
       </left>
       <right style="medium">
-        <color rgb="FF23444F"/>
+        <color rgb="FF274452"/>
       </right>
       <top style="medium">
         <color rgb="FF284856"/>
@@ -10287,7 +10288,7 @@
         <color rgb="FF284457"/>
       </left>
       <right style="medium">
-        <color rgb="FF23444F"/>
+        <color rgb="FF274452"/>
       </right>
       <top style="medium">
         <color rgb="FF284856"/>
@@ -10410,7 +10411,7 @@
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="medium">
-        <color rgb="FF2F4E5E"/>
+        <color rgb="FF2F4D5D"/>
       </right>
       <top style="medium"/>
       <bottom style="medium"/>
@@ -10418,7 +10419,7 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="medium">
-        <color rgb="FF2F4E5E"/>
+        <color rgb="FF2F4D5D"/>
       </left>
       <right style="medium"/>
       <top style="medium"/>
@@ -10451,7 +10452,7 @@
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="medium">
-        <color rgb="FF1C3847"/>
+        <color rgb="FF1C3846"/>
       </right>
       <top style="medium"/>
       <bottom style="medium"/>
@@ -10459,7 +10460,7 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thick">
-        <color rgb="FF0C1E2C"/>
+        <color rgb="FF0C1F2D"/>
       </left>
       <right style="medium">
         <color rgb="FF183848"/>
@@ -10526,17 +10527,6 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="medium">
-        <color rgb="FF183848"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF133445"/>
-      </right>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium">
         <color rgb="FF133445"/>
       </left>
       <right style="medium">
@@ -10565,15 +10555,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium">
-        <color rgb="FF143844"/>
-      </right>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="medium">
         <color rgb="FF183444"/>
       </left>
@@ -10596,7 +10577,7 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="medium">
-        <color rgb="FF1C3847"/>
+        <color rgb="FF1C3846"/>
       </right>
       <top style="medium"/>
       <bottom style="medium"/>
@@ -10749,603 +10730,603 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="50" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="50" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="55" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="55" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="56" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="56" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="58" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="58" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="59" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="59" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="60" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="60" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="61" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="61" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="62" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="62" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="62" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="62" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="63" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="63" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="64" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="64" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="65" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="65" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="64" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="64" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="66" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="66" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="66" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="66" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="63" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="63" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="67" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="64" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="68" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="67" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="69" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="68" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="70" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="69" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="69" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="68" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="71" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="62" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="70" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="69" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="72" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="70" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="73" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="71" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="70" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="69" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="73" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="71" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="74" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="72" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="75" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="73" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="76" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="74" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="77" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="75" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="78" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="76" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="79" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="77" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="80" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="78" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="81" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="79" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="82" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="80" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="83" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="81" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="84" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="82" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="82" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="80" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="85" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="83" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="0" borderId="86" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="84" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11363,57 +11344,57 @@
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FF00020F"/>
       <rgbColor rgb="FF2A4656"/>
-      <rgbColor rgb="FF23444F"/>
+      <rgbColor rgb="FF22495F"/>
       <rgbColor rgb="FF0A212F"/>
       <rgbColor rgb="FF132D3B"/>
-      <rgbColor rgb="FF284452"/>
+      <rgbColor rgb="FF274452"/>
       <rgbColor rgb="FF213D4B"/>
-      <rgbColor rgb="FF0C1E2C"/>
-      <rgbColor rgb="FF2F5465"/>
+      <rgbColor rgb="FF0C1F2D"/>
+      <rgbColor rgb="FF2B4F5F"/>
       <rgbColor rgb="FF081521"/>
-      <rgbColor rgb="FF2F4D5B"/>
+      <rgbColor rgb="FF365666"/>
       <rgbColor rgb="FF1F3B4B"/>
       <rgbColor rgb="FF3B606B"/>
-      <rgbColor rgb="FF28485B"/>
-      <rgbColor rgb="FF3D5C6D"/>
+      <rgbColor rgb="FF284B57"/>
+      <rgbColor rgb="FF426475"/>
       <rgbColor rgb="FF2B4F64"/>
-      <rgbColor rgb="FF355163"/>
+      <rgbColor rgb="FF385767"/>
       <rgbColor rgb="FF000310"/>
       <rgbColor rgb="FF183444"/>
       <rgbColor rgb="FF0E212F"/>
-      <rgbColor rgb="FF284B57"/>
-      <rgbColor rgb="FF34586A"/>
+      <rgbColor rgb="FF284B5C"/>
+      <rgbColor rgb="FF2F5465"/>
       <rgbColor rgb="FF1D4457"/>
       <rgbColor rgb="FF000515"/>
-      <rgbColor rgb="FF223F4D"/>
+      <rgbColor rgb="FF233F4D"/>
       <rgbColor rgb="FF0C212D"/>
+      <rgbColor rgb="FF183848"/>
       <rgbColor rgb="FF1F3B49"/>
-      <rgbColor rgb="FF1C3847"/>
       <rgbColor rgb="FF112633"/>
       <rgbColor rgb="FF3F6274"/>
       <rgbColor rgb="FF0C212F"/>
-      <rgbColor rgb="FF284B5C"/>
+      <rgbColor rgb="FF2F4B64"/>
       <rgbColor rgb="FF183442"/>
       <rgbColor rgb="FF143844"/>
       <rgbColor rgb="FF081C2A"/>
-      <rgbColor rgb="FF22495F"/>
+      <rgbColor rgb="FF28485B"/>
       <rgbColor rgb="FF284457"/>
       <rgbColor rgb="FF2B4B5B"/>
       <rgbColor rgb="FF193746"/>
-      <rgbColor rgb="FF355666"/>
-      <rgbColor rgb="FF2B4F5F"/>
+      <rgbColor rgb="FF345967"/>
+      <rgbColor rgb="FF2F4D5B"/>
       <rgbColor rgb="FF2B4B57"/>
-      <rgbColor rgb="FF183848"/>
+      <rgbColor rgb="FF1C3846"/>
       <rgbColor rgb="FF284856"/>
       <rgbColor rgb="FF2B4857"/>
       <rgbColor rgb="FF446578"/>
-      <rgbColor rgb="FF2F4E5E"/>
+      <rgbColor rgb="FF2F4D5D"/>
       <rgbColor rgb="FF133445"/>
-      <rgbColor rgb="FF385767"/>
+      <rgbColor rgb="FF3D5D6E"/>
       <rgbColor rgb="FF052130"/>
       <rgbColor rgb="FF182733"/>
       <rgbColor rgb="FF2F4B5A"/>
-      <rgbColor rgb="FF2F4B64"/>
+      <rgbColor rgb="FF345260"/>
       <rgbColor rgb="FF2B4860"/>
       <rgbColor rgb="FF233D4D"/>
     </indexedColors>
@@ -11429,7 +11410,7 @@
   <dimension ref="A1:D118"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
se corrige defecto con codigo raro
</commit_message>
<xml_diff>
--- a/app/templates/template_rules_ladder.xlsx
+++ b/app/templates/template_rules_ladder.xlsx
@@ -4883,7 +4883,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">.3,5.11.1.4,5.13.3</t>
+      <t xml:space="preserve">.3</t>
     </r>
   </si>
   <si>
@@ -11409,8 +11409,8 @@
   </sheetPr>
   <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C86" activeCellId="0" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
se añade carpeta 0 a ladder
</commit_message>
<xml_diff>
--- a/app/templates/template_rules_ladder.xlsx
+++ b/app/templates/template_rules_ladder.xlsx
@@ -20,7 +20,76 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="173">
+  <si>
+    <t xml:space="preserve">Certificado conformidad MINVU.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plano de planta ascensores (primer piso).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certificado de inscripción vigente del instalador.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Declaración jurada del instalador, cumple normativa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Declaración jurada del instalador, que se ejecutaron los ensayos y que se encuentra sin fallas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Declaración de instalación eléctrica (te1) y plano respectivo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En ascensores electromecánicos vert. Se adjunta informe técnico.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plano y esp. Técnicas de cada uno anexo c norma 440/1 de los instaladores.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan anual de mantención.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual de procedimiento e inspecciones.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual de uso e instrucciones de rescate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0.11</t>
+  </si>
   <si>
     <r>
       <rPr>
@@ -9527,7 +9596,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="43">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -9558,6 +9627,13 @@
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF1C3846"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color rgb="FF2F4D5D"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -9565,9 +9641,8 @@
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF1C3846"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Calibri"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -9841,17 +9916,17 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="medium"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="medium"/>
       <top style="medium"/>
       <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="medium"/>
-      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -10725,7 +10800,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="153">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -10734,227 +10809,219 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10962,191 +11029,203 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="50" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="50" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="55" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="55" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="56" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="56" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="58" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="26" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="59" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="58" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="60" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="61" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="62" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="62" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="63" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="59" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="60" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="64" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="65" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="61" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="62" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="62" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="63" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="64" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="65" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="64" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="66" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="64" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11154,19 +11233,75 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="63" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="66" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="63" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="64" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="64" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="67" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="67" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="68" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="68" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="69" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="68" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="62" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="69" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="70" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="71" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="69" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="71" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="72" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11174,159 +11309,107 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="69" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="68" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="62" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="73" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="74" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="69" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="75" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="76" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="70" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="77" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="78" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="79" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="80" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="81" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="82" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="71" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="69" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="71" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="80" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="72" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="83" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="73" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="74" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="75" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="76" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="77" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="78" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="79" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="80" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="81" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="82" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="80" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="83" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="41" fillId="0" borderId="84" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="84" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11407,10 +11490,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D118"/>
+  <dimension ref="A1:P129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C86" activeCellId="0" sqref="C86"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11422,1368 +11505,1555 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="7"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>7</v>
+      <c r="A11" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="3"/>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="n">
-        <v>4</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>5</v>
-      </c>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="3"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="3"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="n">
-        <v>5</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>10</v>
+      <c r="A20" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>5</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N20" s="6"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="17"/>
+      <c r="D21" s="9"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="17"/>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N22" s="6"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>5</v>
-      </c>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="5"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="21"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="5"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>5</v>
-      </c>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="5"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="23"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="5"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="22"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="5"/>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N27" s="6"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="27" t="s">
-        <v>2</v>
-      </c>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="16"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="24"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="27"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="16"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="27"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="16"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="28" t="s">
+      <c r="A31" s="17" t="n">
         <v>5</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="24"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="19"/>
     </row>
-    <row r="33" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>2</v>
-      </c>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="17"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="19"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="31" t="n">
-        <v>10</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>2</v>
+      <c r="A34" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="31"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="5"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="23"/>
     </row>
-    <row r="36" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="33" t="n">
-        <v>11</v>
-      </c>
-      <c r="B36" s="25" t="s">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="24"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="24"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="26" t="n">
+        <v>7</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" s="28" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="37" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="33" t="n">
-        <v>12</v>
-      </c>
-      <c r="B37" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>5</v>
-      </c>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="26"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="29"/>
     </row>
-    <row r="38" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38" s="28" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D40" s="28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="B41" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="D41" s="28" t="s">
-        <v>5</v>
-      </c>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="26"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="29"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="B42" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="D42" s="36" t="s">
-        <v>5</v>
+      <c r="A42" s="26" t="n">
+        <v>8</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
+    <row r="44" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="B44" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="37" t="n">
-        <v>16</v>
-      </c>
-      <c r="B45" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="D45" s="40" t="s">
-        <v>2</v>
+      <c r="A45" s="33" t="n">
+        <v>10</v>
+      </c>
+      <c r="B45" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="37"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="40"/>
+      <c r="A46" s="33"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="7"/>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="37"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="40"/>
+    <row r="47" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="35" t="n">
+        <v>11</v>
+      </c>
+      <c r="B47" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="41" t="n">
-        <v>17</v>
-      </c>
-      <c r="B48" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="C48" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="D48" s="44" t="s">
-        <v>44</v>
+    <row r="48" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="35" t="n">
+        <v>12</v>
+      </c>
+      <c r="B48" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="41"/>
-      <c r="B49" s="42"/>
-      <c r="C49" s="43"/>
-      <c r="D49" s="44"/>
+    <row r="49" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="41"/>
-      <c r="B50" s="42"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="44"/>
+    <row r="50" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="41" t="n">
-        <v>18</v>
-      </c>
-      <c r="B51" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="C51" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="D51" s="44" t="s">
-        <v>5</v>
+    <row r="51" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="41"/>
-      <c r="B52" s="42"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="44"/>
+    <row r="52" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="B52" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C52" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="41"/>
-      <c r="B53" s="42"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="44"/>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="B53" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D53" s="38" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="46" t="n">
-        <v>19</v>
-      </c>
-      <c r="B54" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C54" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="D54" s="48" t="s">
-        <v>2</v>
-      </c>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="7"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="38"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="46"/>
-      <c r="B55" s="47"/>
-      <c r="C55" s="46"/>
-      <c r="D55" s="48"/>
+      <c r="A55" s="7"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="46"/>
-      <c r="B56" s="47"/>
-      <c r="C56" s="46"/>
-      <c r="D56" s="48"/>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="39" t="n">
+        <v>16</v>
+      </c>
+      <c r="B56" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" s="42" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="46"/>
-      <c r="B57" s="47"/>
-      <c r="C57" s="46"/>
-      <c r="D57" s="48"/>
+      <c r="A57" s="39"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="42"/>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="49" t="n">
-        <v>20</v>
-      </c>
-      <c r="B58" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="C58" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="D58" s="51" t="s">
-        <v>44</v>
-      </c>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="39"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="41"/>
+      <c r="D58" s="42"/>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="49"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="51"/>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="43" t="n">
+        <v>17</v>
+      </c>
+      <c r="B59" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="D59" s="46" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="49"/>
-      <c r="B60" s="38"/>
-      <c r="C60" s="50"/>
-      <c r="D60" s="51"/>
+      <c r="A60" s="43"/>
+      <c r="B60" s="44"/>
+      <c r="C60" s="45"/>
+      <c r="D60" s="46"/>
     </row>
-    <row r="61" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="41" t="n">
-        <v>21</v>
-      </c>
-      <c r="B61" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="C61" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="D61" s="53" t="s">
-        <v>44</v>
-      </c>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="43"/>
+      <c r="B61" s="44"/>
+      <c r="C61" s="45"/>
+      <c r="D61" s="46"/>
     </row>
-    <row r="62" customFormat="false" ht="116.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="54" t="n">
-        <v>22</v>
-      </c>
-      <c r="B62" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="C62" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="D62" s="57" t="s">
-        <v>2</v>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="43" t="n">
+        <v>18</v>
+      </c>
+      <c r="B62" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="D62" s="46" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="58" t="n">
-        <v>23</v>
-      </c>
-      <c r="B63" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="C63" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="D63" s="57" t="s">
-        <v>44</v>
-      </c>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="43"/>
+      <c r="B63" s="44"/>
+      <c r="C63" s="47"/>
+      <c r="D63" s="46"/>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="54" t="n">
-        <v>24</v>
-      </c>
-      <c r="B64" s="61" t="s">
-        <v>56</v>
-      </c>
-      <c r="C64" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="D64" s="63" t="s">
-        <v>2</v>
-      </c>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="43"/>
+      <c r="B64" s="44"/>
+      <c r="C64" s="47"/>
+      <c r="D64" s="46"/>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="54"/>
-      <c r="B65" s="61"/>
-      <c r="C65" s="62"/>
-      <c r="D65" s="63"/>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="48" t="n">
+        <v>19</v>
+      </c>
+      <c r="B65" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D65" s="50" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="64" t="n">
-        <v>25</v>
-      </c>
-      <c r="B66" s="65" t="s">
-        <v>58</v>
-      </c>
-      <c r="C66" s="66" t="s">
-        <v>59</v>
-      </c>
-      <c r="D66" s="63" t="s">
-        <v>5</v>
-      </c>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="48"/>
+      <c r="B66" s="49"/>
+      <c r="C66" s="48"/>
+      <c r="D66" s="50"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="64"/>
-      <c r="B67" s="65"/>
-      <c r="C67" s="66"/>
-      <c r="D67" s="63"/>
+      <c r="A67" s="48"/>
+      <c r="B67" s="49"/>
+      <c r="C67" s="48"/>
+      <c r="D67" s="50"/>
     </row>
-    <row r="68" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="67" t="n">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="48"/>
+      <c r="B68" s="49"/>
+      <c r="C68" s="48"/>
+      <c r="D68" s="50"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="51" t="n">
+        <v>20</v>
+      </c>
+      <c r="B69" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C69" s="52" t="s">
+        <v>73</v>
+      </c>
+      <c r="D69" s="53" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="51"/>
+      <c r="B70" s="40"/>
+      <c r="C70" s="52"/>
+      <c r="D70" s="53"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="51"/>
+      <c r="B71" s="40"/>
+      <c r="C71" s="52"/>
+      <c r="D71" s="53"/>
+    </row>
+    <row r="72" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="43" t="n">
+        <v>21</v>
+      </c>
+      <c r="B72" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="C72" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="D72" s="55" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="116.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="56" t="n">
+        <v>22</v>
+      </c>
+      <c r="B73" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="D73" s="59" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="60" t="n">
+        <v>23</v>
+      </c>
+      <c r="B74" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="C74" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="D74" s="59" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="56" t="n">
+        <v>24</v>
+      </c>
+      <c r="B75" s="63" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="D75" s="65" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="56"/>
+      <c r="B76" s="63"/>
+      <c r="C76" s="64"/>
+      <c r="D76" s="65"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="66" t="n">
+        <v>25</v>
+      </c>
+      <c r="B77" s="67" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77" s="68" t="s">
+        <v>82</v>
+      </c>
+      <c r="D77" s="65" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="66"/>
+      <c r="B78" s="67"/>
+      <c r="C78" s="68"/>
+      <c r="D78" s="65"/>
+    </row>
+    <row r="79" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="69" t="n">
         <v>26</v>
       </c>
-      <c r="B68" s="68" t="s">
-        <v>60</v>
-      </c>
-      <c r="C68" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="D68" s="69" t="s">
-        <v>2</v>
+      <c r="B79" s="70" t="s">
+        <v>83</v>
+      </c>
+      <c r="C79" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="D79" s="71" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="70" t="n">
+    <row r="80" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="72" t="n">
         <v>27</v>
       </c>
-      <c r="B69" s="71" t="s">
-        <v>62</v>
-      </c>
-      <c r="C69" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="D69" s="72" t="s">
-        <v>64</v>
+      <c r="B80" s="73" t="s">
+        <v>85</v>
+      </c>
+      <c r="C80" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="D80" s="74" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="73" t="n">
+    <row r="81" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="75" t="n">
         <v>28</v>
       </c>
-      <c r="B70" s="71" t="s">
-        <v>65</v>
-      </c>
-      <c r="C70" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="D70" s="72" t="s">
-        <v>66</v>
+      <c r="B81" s="73" t="s">
+        <v>88</v>
+      </c>
+      <c r="C81" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="D81" s="74" t="s">
+        <v>89</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="73" t="n">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="75" t="n">
         <v>29</v>
       </c>
-      <c r="B71" s="74" t="s">
+      <c r="B82" s="76" t="s">
+        <v>90</v>
+      </c>
+      <c r="C82" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="D82" s="75" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="75"/>
+      <c r="B83" s="76"/>
+      <c r="C83" s="66"/>
+      <c r="D83" s="75"/>
+    </row>
+    <row r="84" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="75" t="n">
+        <v>30</v>
+      </c>
+      <c r="B84" s="77" t="s">
+        <v>92</v>
+      </c>
+      <c r="C84" s="66" t="s">
+        <v>93</v>
+      </c>
+      <c r="D84" s="74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="75" t="n">
+        <v>31</v>
+      </c>
+      <c r="B85" s="77" t="s">
+        <v>94</v>
+      </c>
+      <c r="C85" s="66" t="s">
+        <v>95</v>
+      </c>
+      <c r="D85" s="74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="75" t="n">
+        <v>32</v>
+      </c>
+      <c r="B86" s="78" t="s">
+        <v>96</v>
+      </c>
+      <c r="C86" s="75" t="s">
+        <v>97</v>
+      </c>
+      <c r="D86" s="74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="75" t="n">
+        <v>33</v>
+      </c>
+      <c r="B87" s="77" t="s">
+        <v>98</v>
+      </c>
+      <c r="C87" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="D87" s="74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="79" t="n">
+        <v>34</v>
+      </c>
+      <c r="B88" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="C88" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="D88" s="81" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="75" t="n">
+        <v>35</v>
+      </c>
+      <c r="B89" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="C89" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="D89" s="75" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="75"/>
+      <c r="B90" s="82"/>
+      <c r="C90" s="75"/>
+      <c r="D90" s="75"/>
+    </row>
+    <row r="91" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="75" t="n">
+        <v>36</v>
+      </c>
+      <c r="B91" s="73" t="s">
+        <v>104</v>
+      </c>
+      <c r="C91" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="D91" s="74" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="75" t="n">
+        <v>37</v>
+      </c>
+      <c r="B92" s="83" t="s">
+        <v>106</v>
+      </c>
+      <c r="C92" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="D92" s="74" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="75" t="n">
+        <v>38</v>
+      </c>
+      <c r="B93" s="83" t="s">
+        <v>108</v>
+      </c>
+      <c r="C93" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="D93" s="74" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="B94" s="83" t="s">
+        <v>110</v>
+      </c>
+      <c r="C94" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="D94" s="74" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="75" t="s">
+        <v>112</v>
+      </c>
+      <c r="B95" s="83" t="s">
+        <v>113</v>
+      </c>
+      <c r="C95" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="D95" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="C71" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="D71" s="73" t="s">
-        <v>66</v>
-      </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="73"/>
-      <c r="B72" s="74"/>
-      <c r="C72" s="64"/>
-      <c r="D72" s="73"/>
-    </row>
-    <row r="73" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="73" t="n">
-        <v>30</v>
-      </c>
-      <c r="B73" s="75" t="s">
-        <v>69</v>
-      </c>
-      <c r="C73" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="D73" s="72" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="73" t="n">
-        <v>31</v>
-      </c>
-      <c r="B74" s="75" t="s">
-        <v>71</v>
-      </c>
-      <c r="C74" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="D74" s="72" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="73" t="n">
-        <v>32</v>
-      </c>
-      <c r="B75" s="76" t="s">
-        <v>73</v>
-      </c>
-      <c r="C75" s="73" t="s">
-        <v>74</v>
-      </c>
-      <c r="D75" s="72" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="73" t="n">
-        <v>33</v>
-      </c>
-      <c r="B76" s="75" t="s">
-        <v>75</v>
-      </c>
-      <c r="C76" s="72" t="s">
-        <v>76</v>
-      </c>
-      <c r="D76" s="72" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="77" t="n">
-        <v>34</v>
-      </c>
-      <c r="B77" s="78" t="s">
-        <v>77</v>
-      </c>
-      <c r="C77" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="D77" s="79" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="73" t="n">
-        <v>35</v>
-      </c>
-      <c r="B78" s="80" t="s">
-        <v>79</v>
-      </c>
-      <c r="C78" s="73" t="s">
-        <v>80</v>
-      </c>
-      <c r="D78" s="73" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="73"/>
-      <c r="B79" s="80"/>
-      <c r="C79" s="73"/>
-      <c r="D79" s="73"/>
-    </row>
-    <row r="80" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="73" t="n">
-        <v>36</v>
-      </c>
-      <c r="B80" s="71" t="s">
-        <v>81</v>
-      </c>
-      <c r="C80" s="64" t="s">
-        <v>82</v>
-      </c>
-      <c r="D80" s="72" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="73" t="n">
-        <v>37</v>
-      </c>
-      <c r="B81" s="81" t="s">
-        <v>83</v>
-      </c>
-      <c r="C81" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="D81" s="72" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="73" t="n">
-        <v>38</v>
-      </c>
-      <c r="B82" s="81" t="s">
-        <v>85</v>
-      </c>
-      <c r="C82" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="D82" s="72" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="73" t="s">
-        <v>86</v>
-      </c>
-      <c r="B83" s="81" t="s">
-        <v>87</v>
-      </c>
-      <c r="C83" s="72" t="s">
-        <v>88</v>
-      </c>
-      <c r="D83" s="72" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="73" t="s">
-        <v>89</v>
-      </c>
-      <c r="B84" s="81" t="s">
-        <v>90</v>
-      </c>
-      <c r="C84" s="72" t="s">
-        <v>88</v>
-      </c>
-      <c r="D84" s="72" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="73" t="n">
+    <row r="96" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="75" t="n">
         <v>40</v>
       </c>
-      <c r="B85" s="82" t="s">
-        <v>91</v>
-      </c>
-      <c r="C85" s="72" t="s">
-        <v>92</v>
-      </c>
-      <c r="D85" s="72" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="83" t="n">
-        <v>41</v>
-      </c>
-      <c r="B86" s="84" t="s">
-        <v>93</v>
-      </c>
-      <c r="C86" s="85" t="s">
-        <v>94</v>
-      </c>
-      <c r="D86" s="86" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="83"/>
-      <c r="B87" s="84"/>
-      <c r="C87" s="85"/>
-      <c r="D87" s="86"/>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="83"/>
-      <c r="B88" s="84"/>
-      <c r="C88" s="85"/>
-      <c r="D88" s="86"/>
-    </row>
-    <row r="89" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="73" t="s">
-        <v>95</v>
-      </c>
-      <c r="B89" s="82" t="s">
-        <v>96</v>
-      </c>
-      <c r="C89" s="72" t="s">
-        <v>97</v>
-      </c>
-      <c r="D89" s="72" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="73" t="s">
-        <v>98</v>
-      </c>
-      <c r="B90" s="82" t="s">
-        <v>99</v>
-      </c>
-      <c r="C90" s="72" t="s">
-        <v>97</v>
-      </c>
-      <c r="D90" s="72" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="87" t="n">
-        <v>43</v>
-      </c>
-      <c r="B91" s="88" t="s">
-        <v>100</v>
-      </c>
-      <c r="C91" s="89" t="s">
-        <v>101</v>
-      </c>
-      <c r="D91" s="90" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="87"/>
-      <c r="B92" s="91" t="s">
-        <v>102</v>
-      </c>
-      <c r="C92" s="89"/>
-      <c r="D92" s="90"/>
-    </row>
-    <row r="93" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="87"/>
-      <c r="B93" s="92" t="s">
-        <v>103</v>
-      </c>
-      <c r="C93" s="89"/>
-      <c r="D93" s="90"/>
-    </row>
-    <row r="94" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="93" t="s">
-        <v>104</v>
-      </c>
-      <c r="B94" s="94" t="s">
-        <v>105</v>
-      </c>
-      <c r="C94" s="95" t="s">
-        <v>106</v>
-      </c>
-      <c r="D94" s="89" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="116.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="96" t="s">
-        <v>107</v>
-      </c>
-      <c r="B95" s="97" t="s">
-        <v>108</v>
-      </c>
-      <c r="C95" s="98" t="s">
-        <v>109</v>
-      </c>
-      <c r="D95" s="72" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="90" t="n">
-        <v>45</v>
-      </c>
-      <c r="B96" s="99" t="s">
-        <v>110</v>
-      </c>
-      <c r="C96" s="100" t="s">
-        <v>111</v>
-      </c>
-      <c r="D96" s="72" t="s">
-        <v>5</v>
+      <c r="B96" s="84" t="s">
+        <v>114</v>
+      </c>
+      <c r="C96" s="74" t="s">
+        <v>115</v>
+      </c>
+      <c r="D96" s="74" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="101" t="n">
-        <v>46</v>
-      </c>
-      <c r="B97" s="102" t="s">
-        <v>112</v>
-      </c>
-      <c r="C97" s="103" t="s">
-        <v>113</v>
-      </c>
-      <c r="D97" s="73" t="s">
-        <v>2</v>
+      <c r="A97" s="85" t="n">
+        <v>41</v>
+      </c>
+      <c r="B97" s="86" t="s">
+        <v>116</v>
+      </c>
+      <c r="C97" s="87" t="s">
+        <v>117</v>
+      </c>
+      <c r="D97" s="88" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="101"/>
-      <c r="B98" s="102"/>
-      <c r="C98" s="103"/>
-      <c r="D98" s="73"/>
+      <c r="A98" s="85"/>
+      <c r="B98" s="86"/>
+      <c r="C98" s="87"/>
+      <c r="D98" s="88"/>
     </row>
-    <row r="99" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="101" t="n">
-        <v>47</v>
-      </c>
-      <c r="B99" s="104" t="s">
-        <v>114</v>
-      </c>
-      <c r="C99" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="D99" s="72" t="s">
-        <v>2</v>
-      </c>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="85"/>
+      <c r="B99" s="86"/>
+      <c r="C99" s="87"/>
+      <c r="D99" s="88"/>
     </row>
-    <row r="100" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="101" t="n">
-        <v>48</v>
-      </c>
-      <c r="B100" s="104" t="s">
-        <v>116</v>
-      </c>
-      <c r="C100" s="106" t="s">
-        <v>117</v>
-      </c>
-      <c r="D100" s="72" t="s">
-        <v>2</v>
+    <row r="100" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="75" t="s">
+        <v>118</v>
+      </c>
+      <c r="B100" s="84" t="s">
+        <v>119</v>
+      </c>
+      <c r="C100" s="74" t="s">
+        <v>120</v>
+      </c>
+      <c r="D100" s="74" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="107" t="n">
-        <v>49</v>
-      </c>
-      <c r="B101" s="108" t="s">
-        <v>118</v>
-      </c>
-      <c r="C101" s="109" t="s">
-        <v>119</v>
-      </c>
-      <c r="D101" s="109" t="s">
-        <v>5</v>
+    <row r="101" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="75" t="s">
+        <v>121</v>
+      </c>
+      <c r="B101" s="84" t="s">
+        <v>122</v>
+      </c>
+      <c r="C101" s="74" t="s">
+        <v>120</v>
+      </c>
+      <c r="D101" s="74" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="107"/>
-      <c r="B102" s="108"/>
-      <c r="C102" s="109"/>
-      <c r="D102" s="109"/>
+    <row r="102" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="89" t="n">
+        <v>43</v>
+      </c>
+      <c r="B102" s="90" t="s">
+        <v>123</v>
+      </c>
+      <c r="C102" s="91" t="s">
+        <v>124</v>
+      </c>
+      <c r="D102" s="92" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="103" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="110" t="n">
-        <v>50</v>
-      </c>
-      <c r="B103" s="111" t="s">
-        <v>120</v>
-      </c>
-      <c r="C103" s="112" t="s">
-        <v>121</v>
-      </c>
-      <c r="D103" s="113" t="s">
-        <v>44</v>
-      </c>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="89"/>
+      <c r="B103" s="93" t="s">
+        <v>125</v>
+      </c>
+      <c r="C103" s="91"/>
+      <c r="D103" s="92"/>
     </row>
-    <row r="104" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="114" t="n">
-        <v>51</v>
-      </c>
-      <c r="B104" s="115" t="s">
-        <v>122</v>
-      </c>
-      <c r="C104" s="116" t="s">
-        <v>123</v>
-      </c>
-      <c r="D104" s="113" t="s">
-        <v>2</v>
-      </c>
+    <row r="104" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="89"/>
+      <c r="B104" s="94" t="s">
+        <v>126</v>
+      </c>
+      <c r="C104" s="91"/>
+      <c r="D104" s="92"/>
     </row>
-    <row r="105" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="110" t="n">
-        <v>52</v>
-      </c>
-      <c r="B105" s="117" t="s">
-        <v>124</v>
-      </c>
-      <c r="C105" s="116" t="s">
-        <v>125</v>
-      </c>
-      <c r="D105" s="113" t="s">
-        <v>5</v>
+    <row r="105" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="95" t="s">
+        <v>127</v>
+      </c>
+      <c r="B105" s="96" t="s">
+        <v>128</v>
+      </c>
+      <c r="C105" s="97" t="s">
+        <v>129</v>
+      </c>
+      <c r="D105" s="91" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="110" t="n">
-        <v>53</v>
-      </c>
-      <c r="B106" s="118" t="s">
-        <v>126</v>
-      </c>
-      <c r="C106" s="119" t="s">
-        <v>127</v>
-      </c>
-      <c r="D106" s="113" t="s">
-        <v>5</v>
+    <row r="106" customFormat="false" ht="116.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="98" t="s">
+        <v>130</v>
+      </c>
+      <c r="B106" s="99" t="s">
+        <v>131</v>
+      </c>
+      <c r="C106" s="100" t="s">
+        <v>132</v>
+      </c>
+      <c r="D106" s="74" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="110" t="n">
-        <v>54</v>
-      </c>
-      <c r="B107" s="120" t="s">
-        <v>128</v>
-      </c>
-      <c r="C107" s="116" t="s">
-        <v>129</v>
-      </c>
-      <c r="D107" s="113" t="s">
-        <v>5</v>
+    <row r="107" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="92" t="n">
+        <v>45</v>
+      </c>
+      <c r="B107" s="101" t="s">
+        <v>133</v>
+      </c>
+      <c r="C107" s="102" t="s">
+        <v>134</v>
+      </c>
+      <c r="D107" s="74" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="110" t="n">
-        <v>55</v>
-      </c>
-      <c r="B108" s="120" t="s">
-        <v>130</v>
-      </c>
-      <c r="C108" s="121" t="s">
-        <v>131</v>
-      </c>
-      <c r="D108" s="122" t="s">
-        <v>5</v>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A108" s="103" t="n">
+        <v>46</v>
+      </c>
+      <c r="B108" s="104" t="s">
+        <v>135</v>
+      </c>
+      <c r="C108" s="105" t="s">
+        <v>136</v>
+      </c>
+      <c r="D108" s="75" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="123" t="n">
-        <v>56</v>
-      </c>
-      <c r="B109" s="124" t="s">
-        <v>132</v>
-      </c>
-      <c r="C109" s="125" t="s">
-        <v>133</v>
-      </c>
-      <c r="D109" s="112" t="s">
-        <v>2</v>
-      </c>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="103"/>
+      <c r="B109" s="104"/>
+      <c r="C109" s="105"/>
+      <c r="D109" s="75"/>
     </row>
     <row r="110" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="126" t="n">
+      <c r="A110" s="103" t="n">
+        <v>47</v>
+      </c>
+      <c r="B110" s="106" t="s">
+        <v>137</v>
+      </c>
+      <c r="C110" s="107" t="s">
+        <v>138</v>
+      </c>
+      <c r="D110" s="74" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="103" t="n">
+        <v>48</v>
+      </c>
+      <c r="B111" s="106" t="s">
+        <v>139</v>
+      </c>
+      <c r="C111" s="108" t="s">
+        <v>140</v>
+      </c>
+      <c r="D111" s="74" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A112" s="109" t="n">
+        <v>49</v>
+      </c>
+      <c r="B112" s="110" t="s">
+        <v>141</v>
+      </c>
+      <c r="C112" s="111" t="s">
+        <v>142</v>
+      </c>
+      <c r="D112" s="111" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="109"/>
+      <c r="B113" s="110"/>
+      <c r="C113" s="111"/>
+      <c r="D113" s="111"/>
+    </row>
+    <row r="114" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="112" t="n">
+        <v>50</v>
+      </c>
+      <c r="B114" s="113" t="s">
+        <v>143</v>
+      </c>
+      <c r="C114" s="114" t="s">
+        <v>144</v>
+      </c>
+      <c r="D114" s="115" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="116" t="n">
+        <v>51</v>
+      </c>
+      <c r="B115" s="117" t="s">
+        <v>145</v>
+      </c>
+      <c r="C115" s="118" t="s">
+        <v>146</v>
+      </c>
+      <c r="D115" s="115" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="112" t="n">
+        <v>52</v>
+      </c>
+      <c r="B116" s="119" t="s">
+        <v>147</v>
+      </c>
+      <c r="C116" s="118" t="s">
+        <v>148</v>
+      </c>
+      <c r="D116" s="115" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="112" t="n">
+        <v>53</v>
+      </c>
+      <c r="B117" s="120" t="s">
+        <v>149</v>
+      </c>
+      <c r="C117" s="121" t="s">
+        <v>150</v>
+      </c>
+      <c r="D117" s="115" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="112" t="n">
+        <v>54</v>
+      </c>
+      <c r="B118" s="122" t="s">
+        <v>151</v>
+      </c>
+      <c r="C118" s="118" t="s">
+        <v>152</v>
+      </c>
+      <c r="D118" s="115" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="112" t="n">
+        <v>55</v>
+      </c>
+      <c r="B119" s="122" t="s">
+        <v>153</v>
+      </c>
+      <c r="C119" s="123" t="s">
+        <v>154</v>
+      </c>
+      <c r="D119" s="124" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="125" t="n">
+        <v>56</v>
+      </c>
+      <c r="B120" s="126" t="s">
+        <v>155</v>
+      </c>
+      <c r="C120" s="127" t="s">
+        <v>156</v>
+      </c>
+      <c r="D120" s="114" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="128" t="n">
         <v>57</v>
       </c>
-      <c r="B110" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C110" s="128" t="s">
-        <v>135</v>
-      </c>
-      <c r="D110" s="129" t="s">
-        <v>2</v>
+      <c r="B121" s="129" t="s">
+        <v>157</v>
+      </c>
+      <c r="C121" s="130" t="s">
+        <v>158</v>
+      </c>
+      <c r="D121" s="131" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="130" t="n">
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A122" s="132" t="n">
         <v>58</v>
       </c>
-      <c r="B111" s="131" t="s">
-        <v>136</v>
-      </c>
-      <c r="C111" s="132" t="s">
-        <v>137</v>
-      </c>
-      <c r="D111" s="133" t="s">
-        <v>2</v>
+      <c r="B122" s="133" t="s">
+        <v>159</v>
+      </c>
+      <c r="C122" s="134" t="s">
+        <v>160</v>
+      </c>
+      <c r="D122" s="135" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="130"/>
-      <c r="B112" s="131"/>
-      <c r="C112" s="132"/>
-      <c r="D112" s="133"/>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="132"/>
+      <c r="B123" s="133"/>
+      <c r="C123" s="134"/>
+      <c r="D123" s="135"/>
     </row>
-    <row r="113" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="134" t="n">
+    <row r="124" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="136" t="n">
         <v>59</v>
       </c>
-      <c r="B113" s="135" t="s">
-        <v>138</v>
-      </c>
-      <c r="C113" s="136" t="s">
-        <v>139</v>
-      </c>
-      <c r="D113" s="137" t="s">
-        <v>2</v>
+      <c r="B124" s="137" t="s">
+        <v>161</v>
+      </c>
+      <c r="C124" s="138" t="s">
+        <v>162</v>
+      </c>
+      <c r="D124" s="139" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="138" t="n">
+    <row r="125" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="140" t="n">
         <v>60</v>
       </c>
-      <c r="B114" s="139" t="s">
-        <v>140</v>
-      </c>
-      <c r="C114" s="140" t="s">
-        <v>141</v>
-      </c>
-      <c r="D114" s="141" t="s">
-        <v>5</v>
+      <c r="B125" s="141" t="s">
+        <v>163</v>
+      </c>
+      <c r="C125" s="142" t="s">
+        <v>164</v>
+      </c>
+      <c r="D125" s="143" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="116.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="142" t="s">
-        <v>142</v>
-      </c>
-      <c r="B115" s="143" t="s">
-        <v>143</v>
-      </c>
-      <c r="C115" s="144" t="s">
-        <v>144</v>
-      </c>
-      <c r="D115" s="126" t="s">
-        <v>2</v>
+    <row r="126" customFormat="false" ht="116.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="144" t="s">
+        <v>165</v>
+      </c>
+      <c r="B126" s="145" t="s">
+        <v>166</v>
+      </c>
+      <c r="C126" s="146" t="s">
+        <v>167</v>
+      </c>
+      <c r="D126" s="128" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="116.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="142" t="s">
-        <v>145</v>
-      </c>
-      <c r="B116" s="145" t="s">
-        <v>146</v>
-      </c>
-      <c r="C116" s="146" t="s">
-        <v>147</v>
-      </c>
-      <c r="D116" s="147" t="s">
-        <v>5</v>
+    <row r="127" customFormat="false" ht="116.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="144" t="s">
+        <v>168</v>
+      </c>
+      <c r="B127" s="147" t="s">
+        <v>169</v>
+      </c>
+      <c r="C127" s="148" t="s">
+        <v>170</v>
+      </c>
+      <c r="D127" s="149" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="142" t="n">
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A128" s="144" t="n">
         <v>62</v>
       </c>
-      <c r="B117" s="148" t="s">
-        <v>148</v>
-      </c>
-      <c r="C117" s="149" t="s">
-        <v>149</v>
-      </c>
-      <c r="D117" s="150" t="s">
-        <v>44</v>
+      <c r="B128" s="150" t="s">
+        <v>171</v>
+      </c>
+      <c r="C128" s="151" t="s">
+        <v>172</v>
+      </c>
+      <c r="D128" s="152" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="142"/>
-      <c r="B118" s="148"/>
-      <c r="C118" s="149"/>
-      <c r="D118" s="150"/>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="144"/>
+      <c r="B129" s="150"/>
+      <c r="C129" s="151"/>
+      <c r="D129" s="152"/>
     </row>
   </sheetData>
   <mergeCells count="103">
-    <mergeCell ref="A1:A8"/>
-    <mergeCell ref="B1:B8"/>
-    <mergeCell ref="C1:C8"/>
-    <mergeCell ref="D1:D8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="C12:C19"/>
+    <mergeCell ref="D12:D19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="D31:D33"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="D48:D50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="D54:D57"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="D58:D60"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="B86:B88"/>
-    <mergeCell ref="C86:C88"/>
-    <mergeCell ref="D86:D88"/>
-    <mergeCell ref="A91:A93"/>
-    <mergeCell ref="C91:C93"/>
-    <mergeCell ref="D91:D93"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="A101:A102"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="D101:D102"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="B111:B112"/>
-    <mergeCell ref="C111:C112"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="B117:B118"/>
-    <mergeCell ref="C117:C118"/>
-    <mergeCell ref="D117:D118"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="D59:D61"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="C65:C68"/>
+    <mergeCell ref="D65:D68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="D69:D71"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="B97:B99"/>
+    <mergeCell ref="C97:C99"/>
+    <mergeCell ref="D97:D99"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="C102:C104"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="B108:B109"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="B112:B113"/>
+    <mergeCell ref="C112:C113"/>
+    <mergeCell ref="D112:D113"/>
+    <mergeCell ref="A122:A123"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="D122:D123"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="D128:D129"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>